<commit_message>
Uploading excel working 100%
</commit_message>
<xml_diff>
--- a/pene.xlsx
+++ b/pene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Desktop\XTEC-Digital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF61CBE2-E1A8-4E19-979C-D05CC31A7FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E532DF99-639F-48F2-A4B5-D377D2CB6F39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,16 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$B$1:$N$69</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjGw/ylRYRgTT+xZU5+4ftFIJwT1Q=="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Carnet</t>
   </si>
@@ -69,7 +64,28 @@
     <t>Apellido2Profesor</t>
   </si>
   <si>
-    <t>pene</t>
+    <t>CE3101</t>
+  </si>
+  <si>
+    <t>1111-1111</t>
+  </si>
+  <si>
+    <t>Alds</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>dsfa</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>fdds</t>
   </si>
 </sst>
 </file>
@@ -133,10 +149,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -148,9 +165,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8E775780-AA2B-4643-BC0D-EFB60FDC1ECE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -365,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -441,86 +463,60 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7">
+        <v>2018114634</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4">
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7">
+        <v>2000</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
         <v>2</v>
       </c>
-      <c r="D2" s="3">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5">
-        <v>5</v>
-      </c>
-      <c r="G2" s="5">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3">
-        <v>8</v>
-      </c>
-      <c r="J2" s="5">
-        <v>9</v>
-      </c>
-      <c r="K2" s="5">
-        <v>10</v>
-      </c>
-      <c r="L2" s="5">
-        <v>11</v>
-      </c>
-      <c r="M2" s="5">
-        <v>12</v>
-      </c>
-      <c r="N2" s="5">
-        <v>13</v>
+      <c r="K2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4">
-        <v>17</v>
-      </c>
-      <c r="F3" s="5">
-        <v>18</v>
-      </c>
-      <c r="G3" s="5">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3">
-        <v>21</v>
-      </c>
-      <c r="J3" s="5">
-        <v>22</v>
-      </c>
-      <c r="K3" s="5">
-        <v>23</v>
-      </c>
-      <c r="L3" s="5">
-        <v>24</v>
-      </c>
-      <c r="M3" s="5">
-        <v>25</v>
-      </c>
-      <c r="N3" s="5">
-        <v>26</v>
-      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>

</xml_diff>